<commit_message>
update bruker example files
</commit_message>
<xml_diff>
--- a/data/bruker_example_input_9_pt_dr_complex.xlsx
+++ b/data/bruker_example_input_9_pt_dr_complex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apaulson/OrbStack/ubuntu/home/apaulson/repos/Notebooks/SMDC/SMDC_2_pre_screen_analysis/Chad_SPR_plate_formatting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apaulson/OrbStack/ubuntu/home/apaulson/repos/smdc_preprocess_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE1CD2F-12A4-8C44-8CDD-8E116DAAC4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3070B1-8A5A-4648-B869-46F7886944F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{319C735B-FEA9-4FD1-82F8-9196C7FC0DFC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{319C735B-FEA9-4FD1-82F8-9196C7FC0DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="138">
   <si>
     <t>Sample Name</t>
   </si>
@@ -472,13 +472,17 @@
   <si>
     <t>&lt;- your name for file saving</t>
   </si>
+  <si>
+    <t>Middle Concentration (uM)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -654,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -713,6 +717,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1058,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A90E0F-EB22-48B1-9A5A-36849773D290}">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1087,23 +1100,23 @@
     <col min="19" max="19" width="26.1640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1112,7 +1125,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1121,7 +1134,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1130,7 +1143,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>23</v>
       </c>
@@ -1139,7 +1152,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>24</v>
       </c>
@@ -1148,11 +1161,11 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D9" s="4"/>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1186,7 @@
       <c r="R10"/>
       <c r="S10"/>
     </row>
-    <row r="11" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -1216,13 +1229,16 @@
       <c r="N11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Q11" s="11"/>
-      <c r="S11" s="12"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R11" s="11"/>
+      <c r="T11" s="12"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1242,12 +1258,20 @@
         <f t="shared" ref="N12" si="0">IFERROR(L12/M12^8,"")</f>
         <v/>
       </c>
-      <c r="O12" s="9" t="str">
+      <c r="O12" s="23" t="str">
+        <f>IFERROR(L12/M12^4,"")</f>
+        <v/>
+      </c>
+      <c r="P12" s="9" t="str">
         <f>IF(2.5*(H12/400)/100/1000=0,"",2.5*(H12/400)/100/1000)</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q12" s="1"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1288,12 +1312,20 @@
         <f>IFERROR(L13/M13^8,"")</f>
         <v>1.5241579027587259E-2</v>
       </c>
-      <c r="O13" s="9">
-        <f t="shared" ref="O13" si="1">IF(2.5*(H13/400)/100/1000=0,"",2.5*(H13/400)/100/1000)</f>
+      <c r="O13" s="23">
+        <f t="shared" ref="O13:O75" si="1">IFERROR(L13/M13^4,"")</f>
+        <v>1.2345679012345678</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" ref="P13" si="2">IF(2.5*(H13/400)/100/1000=0,"",2.5*(H13/400)/100/1000)</f>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q13" s="1"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1334,12 +1366,20 @@
         <f>IFERROR(L14/M14^8,"")</f>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P14" s="9">
         <f>IF(2.5*(H14/400)/100/1000=0,"",2.5*(H14/400)/100/1000)</f>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1377,15 +1417,23 @@
         <v>2</v>
       </c>
       <c r="N15" s="17">
-        <f t="shared" ref="N15:N18" si="2">IFERROR(L15/M15^8,"")</f>
+        <f t="shared" ref="N15:N18" si="3">IFERROR(L15/M15^8,"")</f>
         <v>3.90625E-2</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="23">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+      <c r="P15" s="9">
         <f>IF(2.5*(H15/400)/100/1000=0,"",2.5*(H15/400)/100/1000)</f>
         <v>3.1250000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1402,15 +1450,23 @@
         <v>35</v>
       </c>
       <c r="N16" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O16" s="9" t="str">
-        <f t="shared" ref="O16:O75" si="3">IF(2.5*(H16/400)/100/1000=0,"",2.5*(H16/400)/100/1000)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O16" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P16" s="9" t="str">
+        <f t="shared" ref="P16:P75" si="4">IF(2.5*(H16/400)/100/1000=0,"",2.5*(H16/400)/100/1000)</f>
+        <v/>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1451,12 +1507,20 @@
         <f>IFERROR(L17/M17^8,"")</f>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O17" s="9">
-        <f t="shared" si="3"/>
+      <c r="O17" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P17" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1495,15 +1559,23 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="N18" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.011291503906252</v>
       </c>
-      <c r="O18" s="9">
-        <f t="shared" si="3"/>
+      <c r="O18" s="23">
+        <f t="shared" si="1"/>
+        <v>31.640625</v>
+      </c>
+      <c r="P18" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1544,12 +1616,20 @@
         <f>IFERROR(L19/M19^8,"")</f>
         <v>3.90625E-2</v>
       </c>
-      <c r="O19" s="9">
-        <f t="shared" si="3"/>
+      <c r="O19" s="23">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+      <c r="P19" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1566,15 +1646,23 @@
         <v>35</v>
       </c>
       <c r="N20" s="17" t="str">
-        <f t="shared" ref="N20:N75" si="4">IFERROR(L20/M20^8,"")</f>
-        <v/>
-      </c>
-      <c r="O20" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="N20:N75" si="5">IFERROR(L20/M20^8,"")</f>
+        <v/>
+      </c>
+      <c r="O20" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P20" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1612,15 +1700,23 @@
         <v>2</v>
       </c>
       <c r="N21" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.90625E-3</v>
       </c>
-      <c r="O21" s="9">
-        <f t="shared" si="3"/>
+      <c r="O21" s="23">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="P21" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q21" s="1"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1658,15 +1754,23 @@
         <v>1.8</v>
       </c>
       <c r="N22" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.0744426271167065E-4</v>
       </c>
-      <c r="O22" s="9">
-        <f t="shared" si="3"/>
+      <c r="O22" s="23">
+        <f t="shared" si="1"/>
+        <v>9.5259868922420356E-3</v>
+      </c>
+      <c r="P22" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="10"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1704,15 +1808,23 @@
         <v>1.01</v>
       </c>
       <c r="N23" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.234832224823122E-4</v>
       </c>
-      <c r="O23" s="9">
-        <f t="shared" si="3"/>
+      <c r="O23" s="23">
+        <f t="shared" si="1"/>
+        <v>9.6098034448281625E-4</v>
+      </c>
+      <c r="P23" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q23" s="1"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1729,15 +1841,23 @@
         <v>35</v>
       </c>
       <c r="N24" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O24" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O24" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P24" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1775,15 +1895,23 @@
         <v>4</v>
       </c>
       <c r="N25" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O25" s="9">
-        <f t="shared" si="3"/>
+      <c r="O25" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P25" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q25" s="1"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="10"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1797,15 +1925,23 @@
         <v>15</v>
       </c>
       <c r="N26" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O26" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O26" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P26" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="10"/>
+    </row>
+    <row r="27" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1843,15 +1979,23 @@
         <v>4</v>
       </c>
       <c r="N27" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O27" s="9">
-        <f t="shared" si="3"/>
+      <c r="O27" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P27" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q27" s="1"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1868,15 +2012,23 @@
         <v>35</v>
       </c>
       <c r="N28" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O28" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O28" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P28" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="10"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1890,15 +2042,23 @@
         <v>18</v>
       </c>
       <c r="N29" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O29" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O29" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P29" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="10"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1912,15 +2072,23 @@
         <v>19</v>
       </c>
       <c r="N30" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O30" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O30" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P30" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="10"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1934,15 +2102,23 @@
         <v>20</v>
       </c>
       <c r="N31" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O31" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O31" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P31" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="10"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1959,15 +2135,23 @@
         <v>35</v>
       </c>
       <c r="N32" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O32" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O32" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P32" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="10"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1981,15 +2165,23 @@
         <v>22</v>
       </c>
       <c r="N33" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O33" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O33" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P33" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="10"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2003,15 +2195,23 @@
         <v>23</v>
       </c>
       <c r="N34" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O34" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O34" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P34" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="10"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2025,15 +2225,23 @@
         <v>24</v>
       </c>
       <c r="N35" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O35" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O35" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P35" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="10"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2050,15 +2258,23 @@
         <v>35</v>
       </c>
       <c r="N36" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O36" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O36" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P36" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="10"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2096,15 +2312,23 @@
         <v>4</v>
       </c>
       <c r="N37" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.373291015625E-3</v>
       </c>
-      <c r="O37" s="9">
-        <f t="shared" si="3"/>
+      <c r="O37" s="23">
+        <f t="shared" si="1"/>
+        <v>0.3515625</v>
+      </c>
+      <c r="P37" s="9">
+        <f t="shared" si="4"/>
         <v>5.6249999999999996E-4</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q37" s="1"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="10"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2142,15 +2366,23 @@
         <v>4</v>
       </c>
       <c r="N38" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O38" s="9">
-        <f t="shared" si="3"/>
+      <c r="O38" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P38" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q38" s="1"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="10"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2188,15 +2420,23 @@
         <v>4</v>
       </c>
       <c r="N39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O39" s="9">
-        <f t="shared" si="3"/>
+      <c r="O39" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P39" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q39" s="1"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="10"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2213,15 +2453,23 @@
         <v>35</v>
       </c>
       <c r="N40" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O40" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O40" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P40" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="10"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2235,15 +2483,23 @@
         <v>30</v>
       </c>
       <c r="N41" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O41" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O41" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P41" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="10"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2257,15 +2513,23 @@
         <v>31</v>
       </c>
       <c r="N42" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O42" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O42" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P42" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="10"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>1</v>
       </c>
@@ -2283,15 +2547,23 @@
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O43" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O43" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P43" s="19" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="10"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -2330,15 +2602,23 @@
         <v>4</v>
       </c>
       <c r="N44" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O44" s="9">
-        <f t="shared" si="3"/>
+      <c r="O44" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P44" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q44" s="1"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="10"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2376,15 +2656,23 @@
         <v>4</v>
       </c>
       <c r="N45" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O45" s="9">
-        <f t="shared" si="3"/>
+      <c r="O45" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P45" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q45" s="1"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="10"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -2422,15 +2710,23 @@
         <v>4</v>
       </c>
       <c r="N46" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O46" s="9">
-        <f t="shared" si="3"/>
+      <c r="O46" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P46" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q46" s="1"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="10"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2468,15 +2764,23 @@
         <v>4</v>
       </c>
       <c r="N47" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O47" s="9">
-        <f t="shared" si="3"/>
+      <c r="O47" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P47" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q47" s="1"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="10"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2514,15 +2818,23 @@
         <v>4</v>
       </c>
       <c r="N48" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O48" s="9">
-        <f t="shared" si="3"/>
+      <c r="O48" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P48" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q48" s="1"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="10"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2560,15 +2872,23 @@
         <v>4</v>
       </c>
       <c r="N49" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O49" s="9">
-        <f t="shared" si="3"/>
+      <c r="O49" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P49" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q49" s="1"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="10"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -2606,15 +2926,23 @@
         <v>4</v>
       </c>
       <c r="N50" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O50" s="9">
-        <f t="shared" si="3"/>
+      <c r="O50" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P50" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q50" s="1"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="10"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2652,15 +2980,23 @@
         <v>4</v>
       </c>
       <c r="N51" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O51" s="9">
-        <f t="shared" si="3"/>
+      <c r="O51" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P51" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q51" s="1"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="10"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -2698,15 +3034,23 @@
         <v>4</v>
       </c>
       <c r="N52" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O52" s="9">
-        <f t="shared" si="3"/>
+      <c r="O52" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P52" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q52" s="1"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="10"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -2744,15 +3088,23 @@
         <v>4</v>
       </c>
       <c r="N53" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O53" s="9">
-        <f t="shared" si="3"/>
+      <c r="O53" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P53" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q53" s="1"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="10"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -2790,15 +3142,23 @@
         <v>4</v>
       </c>
       <c r="N54" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O54" s="9">
-        <f t="shared" si="3"/>
+      <c r="O54" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P54" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q54" s="1"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="10"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -2836,15 +3196,23 @@
         <v>4</v>
       </c>
       <c r="N55" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O55" s="9">
-        <f t="shared" si="3"/>
+      <c r="O55" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P55" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q55" s="1"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="10"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -2882,15 +3250,23 @@
         <v>4</v>
       </c>
       <c r="N56" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O56" s="9">
-        <f t="shared" si="3"/>
+      <c r="O56" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P56" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q56" s="1"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="10"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -2928,15 +3304,23 @@
         <v>4</v>
       </c>
       <c r="N57" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O57" s="9">
-        <f t="shared" si="3"/>
+      <c r="O57" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P57" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q57" s="1"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="10"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -2950,15 +3334,23 @@
         <v>39</v>
       </c>
       <c r="N58" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O58" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O58" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P58" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="10"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -2996,15 +3388,23 @@
         <v>4</v>
       </c>
       <c r="N59" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.52587890625E-3</v>
       </c>
-      <c r="O59" s="9">
-        <f t="shared" si="3"/>
+      <c r="O59" s="23">
+        <f t="shared" si="1"/>
+        <v>0.390625</v>
+      </c>
+      <c r="P59" s="9">
+        <f t="shared" si="4"/>
         <v>6.2500000000000001E-4</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q59" s="1"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="10"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -3018,15 +3418,23 @@
         <v>41</v>
       </c>
       <c r="N60" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O60" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O60" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P60" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="10"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -3040,15 +3448,23 @@
         <v>42</v>
       </c>
       <c r="N61" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O61" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O61" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P61" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="10"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -3062,15 +3478,23 @@
         <v>43</v>
       </c>
       <c r="N62" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O62" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O62" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P62" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="10"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -3084,15 +3508,23 @@
         <v>44</v>
       </c>
       <c r="N63" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O63" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O63" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P63" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="10"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -3106,15 +3538,23 @@
         <v>45</v>
       </c>
       <c r="N64" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O64" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O64" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P64" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="10"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -3128,15 +3568,23 @@
         <v>46</v>
       </c>
       <c r="N65" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O65" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O65" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P65" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="10"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -3150,15 +3598,23 @@
         <v>47</v>
       </c>
       <c r="N66" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O66" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O66" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P66" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="10"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -3172,15 +3628,23 @@
         <v>48</v>
       </c>
       <c r="N67" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O67" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O67" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P67" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="10"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
@@ -3218,15 +3682,23 @@
         <v>3</v>
       </c>
       <c r="N68" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.6207895137936294E-3</v>
       </c>
-      <c r="O68" s="9">
-        <f t="shared" si="3"/>
+      <c r="O68" s="23">
+        <f t="shared" si="1"/>
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="P68" s="9">
+        <f t="shared" si="4"/>
         <v>3.1250000000000001E-4</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q68" s="1"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="10"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2</v>
       </c>
@@ -3264,15 +3736,23 @@
         <v>4</v>
       </c>
       <c r="N69" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.57763671875E-4</v>
       </c>
-      <c r="O69" s="9">
-        <f t="shared" si="3"/>
+      <c r="O69" s="23">
+        <f t="shared" si="1"/>
+        <v>0.1171875</v>
+      </c>
+      <c r="P69" s="9">
+        <f t="shared" si="4"/>
         <v>1.875E-4</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q69" s="1"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="10"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2</v>
       </c>
@@ -3286,15 +3766,23 @@
         <v>51</v>
       </c>
       <c r="N70" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O70" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O70" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P70" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="10"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2</v>
       </c>
@@ -3308,15 +3796,23 @@
         <v>52</v>
       </c>
       <c r="N71" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O71" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O71" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P71" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="10"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
@@ -3330,15 +3826,23 @@
         <v>53</v>
       </c>
       <c r="N72" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O72" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O72" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P72" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="10"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2</v>
       </c>
@@ -3352,15 +3856,23 @@
         <v>54</v>
       </c>
       <c r="N73" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O73" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O73" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P73" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="10"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2</v>
       </c>
@@ -3374,15 +3886,23 @@
         <v>55</v>
       </c>
       <c r="N74" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O74" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O74" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P74" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="10"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>2</v>
       </c>
@@ -3405,13 +3925,21 @@
       <c r="L75" s="5"/>
       <c r="M75" s="5"/>
       <c r="N75" s="18" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O75" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O75" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P75" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3427,11 +3955,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:M75">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>AND(M12&gt;0,N12&gt;=O12,L12&gt;0,(H12)/100&gt;=L12)</formula>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>AND(M12&gt;0,N12&gt;=P12,L12&gt;0,(H12)/100&gt;=L12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>OR(N12&lt;O12,(H12)/100&lt;L12)</formula>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>OR(N12&lt;P12,(H12)/100&lt;L12)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>